<commit_message>
Support import muilply work basises.
</commit_message>
<xml_diff>
--- a/sql/excel/csims系统权限表.xlsx
+++ b/sql/excel/csims系统权限表.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmall\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="21510" windowHeight="10350"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21510" windowHeight="10350"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="261">
   <si>
     <t>ID</t>
   </si>
@@ -743,19 +748,67 @@
   </si>
   <si>
     <t>displayFeedbackExcel</t>
+  </si>
+  <si>
+    <t>toSiftPage</t>
+  </si>
+  <si>
+    <t>siftAePeoples</t>
+  </si>
+  <si>
+    <t>siftAeedOrg</t>
+  </si>
+  <si>
+    <t>toAdminEnforceInitPageFromSift</t>
+  </si>
+  <si>
+    <t>toSiftResultList</t>
+  </si>
+  <si>
+    <t>toAdminEnforceInitPageFromSiftResult</t>
+  </si>
+  <si>
+    <t>generateDesktopClientInitialFile</t>
+  </si>
+  <si>
+    <t>toImportDesktopClientFinalData</t>
+  </si>
+  <si>
+    <t>importDesktopClientFinalData</t>
+  </si>
+  <si>
+    <t>导入行政执法的工作检查记录单机版数据</t>
+  </si>
+  <si>
+    <t>跳转行政执法的工作检查记录单机版数据导入界面</t>
+  </si>
+  <si>
+    <t>导出单机版初始化文件</t>
+  </si>
+  <si>
+    <t>从筛选结果跳转行政执法登记页面</t>
+  </si>
+  <si>
+    <t>筛选结果列表页面</t>
+  </si>
+  <si>
+    <t>保存筛选结果</t>
+  </si>
+  <si>
+    <t>筛选被检查机构</t>
+  </si>
+  <si>
+    <t>筛选其他组成员</t>
+  </si>
+  <si>
+    <t>跳转到筛选执法人员和被检查机构页面</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -776,8 +829,16 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="9"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -810,27 +871,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -846,15 +892,91 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -866,7 +988,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="C7EDCC"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1153,6 +1275,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -1185,15 +1308,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
-  <dimension ref="A1:G117"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117:G126"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="52.625" customWidth="1"/>
     <col min="4" max="4" width="33.125" customWidth="1"/>
@@ -1201,7 +1323,7 @@
     <col min="6" max="6" width="33.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1224,7 +1346,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2">
         <v>200</v>
       </c>
@@ -1248,7 +1370,7 @@
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (200, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政执法检查情况统计表统计页面','/AdminEnforceManagerAction.do?method=toAeinspectionAnl&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3">
         <v>201</v>
       </c>
@@ -1272,7 +1394,7 @@
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (201, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成行政执法检查情况统计表Excel文件','/AdminEnforceManagerAction.do?method=generateAeinspectionAnlExcel&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>202</v>
       </c>
@@ -1296,7 +1418,7 @@
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (202, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政执法登记页面','/AdminEnforceManagerAction.do?method=toAdminEnforceInitPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>203</v>
       </c>
@@ -1320,7 +1442,7 @@
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (203, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政执法登记保存','/AdminEnforceManagerAction.do?method=createAdminEnforce&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>204</v>
       </c>
@@ -1344,7 +1466,7 @@
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (204, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政执法信息列表页面','/AdminEnforceManagerAction.do?method=toAdminEnforceList&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>205</v>
       </c>
@@ -1364,11 +1486,11 @@
         <v>10</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" ref="G7:G35" si="4">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A7&amp;", '"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;F7&amp;"?method="&amp;D7&amp;"&amp;*,ANY',"&amp;E7&amp;");"</f>
+        <f t="shared" ref="G7" si="4">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A7&amp;", '"&amp;B7&amp;"','"&amp;C7&amp;"','"&amp;F7&amp;"?method="&amp;D7&amp;"&amp;*,ANY',"&amp;E7&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (205, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政执法信息详细页面','/AdminEnforceManagerAction.do?method=toAdminEnforceDetailPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>206</v>
       </c>
@@ -1388,11 +1510,11 @@
         <v>10</v>
       </c>
       <c r="G8" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A8&amp;", '"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;F8&amp;"?method="&amp;D8&amp;"&amp;*,ANY',"&amp;E8&amp;");"</f>
+        <f t="shared" ref="G8:G35" si="5">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A8&amp;", '"&amp;B8&amp;"','"&amp;C8&amp;"','"&amp;F8&amp;"?method="&amp;D8&amp;"&amp;*,ANY',"&amp;E8&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (206, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政执法信息修改页面','/AdminEnforceManagerAction.do?method=toUpdateAdminEnforcePage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>207</v>
       </c>
@@ -1412,11 +1534,11 @@
         <v>10</v>
       </c>
       <c r="G9" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A9&amp;", '"&amp;B9&amp;"','"&amp;C9&amp;"','"&amp;F9&amp;"?method="&amp;D9&amp;"&amp;*,ANY',"&amp;E9&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (207, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政执法信息修改','/AdminEnforceManagerAction.do?method=updateAdminEnforce&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="2">
         <v>208</v>
       </c>
@@ -1436,11 +1558,11 @@
         <v>10</v>
       </c>
       <c r="G10" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A10&amp;", '"&amp;B10&amp;"','"&amp;C10&amp;"','"&amp;F10&amp;"?method="&amp;D10&amp;"&amp;*,ANY',"&amp;E10&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (208, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政执法信息删除','/AdminEnforceManagerAction.do?method=delAdminEnforce&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>209</v>
       </c>
@@ -1460,11 +1582,11 @@
         <v>10</v>
       </c>
       <c r="G11" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A11&amp;", '"&amp;B11&amp;"','"&amp;C11&amp;"','"&amp;F11&amp;"?method="&amp;D11&amp;"&amp;*,ANY',"&amp;E11&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (209, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查工作记录录入页面','/AdminEnforceManagerAction.do?method=toAeinspectionInitPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>210</v>
       </c>
@@ -1484,11 +1606,11 @@
         <v>10</v>
       </c>
       <c r="G12" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A12&amp;", '"&amp;B12&amp;"','"&amp;C12&amp;"','"&amp;F12&amp;"?method="&amp;D12&amp;"&amp;*,ANY',"&amp;E12&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (210, 'net.sf.jguard.core.authorization.permissions.URLPermission','检查工作记录保存方法','/AdminEnforceManagerAction.do?method=createAeinspection&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>211</v>
       </c>
@@ -1508,11 +1630,11 @@
         <v>10</v>
       </c>
       <c r="G13" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A13&amp;", '"&amp;B13&amp;"','"&amp;C13&amp;"','"&amp;F13&amp;"?method="&amp;D13&amp;"&amp;*,ANY',"&amp;E13&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (211, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存工作底稿','/AdminEnforceManagerAction.do?method=saveBasis&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>212</v>
       </c>
@@ -1532,11 +1654,11 @@
         <v>10</v>
       </c>
       <c r="G14" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A14&amp;", '"&amp;B14&amp;"','"&amp;C14&amp;"','"&amp;F14&amp;"?method="&amp;D14&amp;"&amp;*,ANY',"&amp;E14&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (212, 'net.sf.jguard.core.authorization.permissions.URLPermission','查询工作底稿','/AdminEnforceManagerAction.do?method=queryBasises&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>213</v>
       </c>
@@ -1556,11 +1678,11 @@
         <v>10</v>
       </c>
       <c r="G15" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A15&amp;", '"&amp;B15&amp;"','"&amp;C15&amp;"','"&amp;F15&amp;"?method="&amp;D15&amp;"&amp;*,ANY',"&amp;E15&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (213, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询工作底稿','/AdminEnforceManagerAction.do?method=pageBasises&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>214</v>
       </c>
@@ -1580,11 +1702,11 @@
         <v>10</v>
       </c>
       <c r="G16" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A16&amp;", '"&amp;B16&amp;"','"&amp;C16&amp;"','"&amp;F16&amp;"?method="&amp;D16&amp;"&amp;*,ANY',"&amp;E16&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (214, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取工作底稿检查详情','/AdminEnforceManagerAction.do?method=getBasisContent&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>215</v>
       </c>
@@ -1604,11 +1726,11 @@
         <v>10</v>
       </c>
       <c r="G17" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A17&amp;", '"&amp;B17&amp;"','"&amp;C17&amp;"','"&amp;F17&amp;"?method="&amp;D17&amp;"&amp;*,ANY',"&amp;E17&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (215, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存进场记录','/AdminEnforceManagerAction.do?method=saveComing&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>216</v>
       </c>
@@ -1628,11 +1750,11 @@
         <v>10</v>
       </c>
       <c r="G18" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A18&amp;", '"&amp;B18&amp;"','"&amp;C18&amp;"','"&amp;F18&amp;"?method="&amp;D18&amp;"&amp;*,ANY',"&amp;E18&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (216, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询进场记录','/AdminEnforceManagerAction.do?method=pageComings&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>217</v>
       </c>
@@ -1652,11 +1774,11 @@
         <v>10</v>
       </c>
       <c r="G19" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A19&amp;", '"&amp;B19&amp;"','"&amp;C19&amp;"','"&amp;F19&amp;"?method="&amp;D19&amp;"&amp;*,ANY',"&amp;E19&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (217, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取进场记录检查详情','/AdminEnforceManagerAction.do?method=getComingContent&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>218</v>
       </c>
@@ -1676,11 +1798,11 @@
         <v>10</v>
       </c>
       <c r="G20" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A20&amp;", '"&amp;B20&amp;"','"&amp;C20&amp;"','"&amp;F20&amp;"?method="&amp;D20&amp;"&amp;*,ANY',"&amp;E20&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (218, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存离场记录','/AdminEnforceManagerAction.do?method=saveGoaway&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>219</v>
       </c>
@@ -1700,11 +1822,11 @@
         <v>10</v>
       </c>
       <c r="G21" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A21&amp;", '"&amp;B21&amp;"','"&amp;C21&amp;"','"&amp;F21&amp;"?method="&amp;D21&amp;"&amp;*,ANY',"&amp;E21&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (219, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询离场记录','/AdminEnforceManagerAction.do?method=pageGoaways&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>220</v>
       </c>
@@ -1724,11 +1846,11 @@
         <v>10</v>
       </c>
       <c r="G22" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A22&amp;", '"&amp;B22&amp;"','"&amp;C22&amp;"','"&amp;F22&amp;"?method="&amp;D22&amp;"&amp;*,ANY',"&amp;E22&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (220, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取离场记录检查详情','/AdminEnforceManagerAction.do?method=getGoawayContent&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>221</v>
       </c>
@@ -1748,11 +1870,11 @@
         <v>10</v>
       </c>
       <c r="G23" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A23&amp;", '"&amp;B23&amp;"','"&amp;C23&amp;"','"&amp;F23&amp;"?method="&amp;D23&amp;"&amp;*,ANY',"&amp;E23&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (221, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存会谈纪要','/AdminEnforceManagerAction.do?method=saveTalkSummary&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>222</v>
       </c>
@@ -1772,11 +1894,11 @@
         <v>10</v>
       </c>
       <c r="G24" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A24&amp;", '"&amp;B24&amp;"','"&amp;C24&amp;"','"&amp;F24&amp;"?method="&amp;D24&amp;"&amp;*,ANY',"&amp;E24&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (222, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询会谈纪要','/AdminEnforceManagerAction.do?method=pageTalkSummarys&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>223</v>
       </c>
@@ -1796,11 +1918,11 @@
         <v>10</v>
       </c>
       <c r="G25" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A25&amp;", '"&amp;B25&amp;"','"&amp;C25&amp;"','"&amp;F25&amp;"?method="&amp;D25&amp;"&amp;*,ANY',"&amp;E25&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (223, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取会谈纪要检查详情','/AdminEnforceManagerAction.do?method=getTalkSummaryContent&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>224</v>
       </c>
@@ -1820,11 +1942,11 @@
         <v>10</v>
       </c>
       <c r="G26" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A26&amp;", '"&amp;B26&amp;"','"&amp;C26&amp;"','"&amp;F26&amp;"?method="&amp;D26&amp;"&amp;*,ANY',"&amp;E26&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (224, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取问题概况树','/AdminEnforceManagerAction.do?method=getProblemSummay&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>225</v>
       </c>
@@ -1844,11 +1966,11 @@
         <v>10</v>
       </c>
       <c r="G27" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A27&amp;", '"&amp;B27&amp;"','"&amp;C27&amp;"','"&amp;F27&amp;"?method="&amp;D27&amp;"&amp;*,ANY',"&amp;E27&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (225, 'net.sf.jguard.core.authorization.permissions.URLPermission','根据选择的问题概况生成事实认定书内容','/AdminEnforceManagerAction.do?method=generateFactBook&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>226</v>
       </c>
@@ -1868,11 +1990,11 @@
         <v>10</v>
       </c>
       <c r="G28" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A28&amp;", '"&amp;B28&amp;"','"&amp;C28&amp;"','"&amp;F28&amp;"?method="&amp;D28&amp;"&amp;*,ANY',"&amp;E28&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (226, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存事实认定书内容','/AdminEnforceManagerAction.do?method=saveFactBook&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>227</v>
       </c>
@@ -1892,11 +2014,11 @@
         <v>10</v>
       </c>
       <c r="G29" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A29&amp;", '"&amp;B29&amp;"','"&amp;C29&amp;"','"&amp;F29&amp;"?method="&amp;D29&amp;"&amp;*,ANY',"&amp;E29&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (227, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存执法统计情况','/AdminEnforceManagerAction.do?method=saveInspectionAnl&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>228</v>
       </c>
@@ -1916,11 +2038,11 @@
         <v>10</v>
       </c>
       <c r="G30" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A30&amp;", '"&amp;B30&amp;"','"&amp;C30&amp;"','"&amp;F30&amp;"?method="&amp;D30&amp;"&amp;*,ANY',"&amp;E30&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (228, 'net.sf.jguard.core.authorization.permissions.URLPermission','查询执法统计情况','/AdminEnforceManagerAction.do?method=pageInspectionAnl&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>229</v>
       </c>
@@ -1940,11 +2062,11 @@
         <v>10</v>
       </c>
       <c r="G31" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A31&amp;", '"&amp;B31&amp;"','"&amp;C31&amp;"','"&amp;F31&amp;"?method="&amp;D31&amp;"&amp;*,ANY',"&amp;E31&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (229, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成事实认定书Word文件','/AdminEnforceManagerAction.do?method=generateWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>230</v>
       </c>
@@ -1964,11 +2086,11 @@
         <v>10</v>
       </c>
       <c r="G32" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A32&amp;", '"&amp;B32&amp;"','"&amp;C32&amp;"','"&amp;F32&amp;"?method="&amp;D32&amp;"&amp;*,ANY',"&amp;E32&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (230, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成工作底稿Word文件','/AdminEnforceManagerAction.do?method=generateGzdgWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>231</v>
       </c>
@@ -1988,11 +2110,11 @@
         <v>10</v>
       </c>
       <c r="G33" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A33&amp;", '"&amp;B33&amp;"','"&amp;C33&amp;"','"&amp;F33&amp;"?method="&amp;D33&amp;"&amp;*,ANY',"&amp;E33&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (231, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成进场记录Word文件','/AdminEnforceManagerAction.do?method=generateJcjlWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>232</v>
       </c>
@@ -2012,11 +2134,11 @@
         <v>10</v>
       </c>
       <c r="G34" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A34&amp;", '"&amp;B34&amp;"','"&amp;C34&amp;"','"&amp;F34&amp;"?method="&amp;D34&amp;"&amp;*,ANY',"&amp;E34&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (232, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成离场会谈记录Word文件','/AdminEnforceManagerAction.do?method=generateLchtjlWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>233</v>
       </c>
@@ -2036,11 +2158,11 @@
         <v>10</v>
       </c>
       <c r="G35" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A35&amp;", '"&amp;B35&amp;"','"&amp;C35&amp;"','"&amp;F35&amp;"?method="&amp;D35&amp;"&amp;*,ANY',"&amp;E35&amp;");"</f>
+        <f t="shared" si="5"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (233, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成会谈纪要Word文件','/AdminEnforceManagerAction.do?method=generateHtjyWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>234</v>
       </c>
@@ -2060,11 +2182,11 @@
         <v>10</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" ref="G36" si="5">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A36&amp;", '"&amp;B36&amp;"','"&amp;C36&amp;"','"&amp;F36&amp;"?method="&amp;D36&amp;"&amp;*,ANY',"&amp;E36&amp;");"</f>
+        <f t="shared" ref="G36" si="6">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A36&amp;", '"&amp;B36&amp;"','"&amp;C36&amp;"','"&amp;F36&amp;"?method="&amp;D36&amp;"&amp;*,ANY',"&amp;E36&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (234, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成立项审批表Word文件','/AdminEnforceManagerAction.do?method=generateLxspbWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>235</v>
       </c>
@@ -2084,11 +2206,11 @@
         <v>10</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" ref="G37" si="6">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A37&amp;", '"&amp;B37&amp;"','"&amp;C37&amp;"','"&amp;F37&amp;"?method="&amp;D37&amp;"&amp;*,ANY',"&amp;E37&amp;");"</f>
+        <f t="shared" ref="G37" si="7">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A37&amp;", '"&amp;B37&amp;"','"&amp;C37&amp;"','"&amp;F37&amp;"?method="&amp;D37&amp;"&amp;*,ANY',"&amp;E37&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (235, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查工作记录列表页面','/AdminEnforceManagerAction.do?method=toAeinspectionList&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>236</v>
       </c>
@@ -2108,11 +2230,11 @@
         <v>10</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" ref="G38" si="7">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A38&amp;", '"&amp;B38&amp;"','"&amp;C38&amp;"','"&amp;F38&amp;"?method="&amp;D38&amp;"&amp;*,ANY',"&amp;E38&amp;");"</f>
+        <f t="shared" ref="G38" si="8">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A38&amp;", '"&amp;B38&amp;"','"&amp;C38&amp;"','"&amp;F38&amp;"?method="&amp;D38&amp;"&amp;*,ANY',"&amp;E38&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (236, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询执法检查情况统计表','/AdminEnforceManagerAction.do?method=pageAeInspectionAnalyse&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>237</v>
       </c>
@@ -2132,11 +2254,11 @@
         <v>10</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" ref="G39:G66" si="8">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A39&amp;", '"&amp;B39&amp;"','"&amp;C39&amp;"','"&amp;F39&amp;"?method="&amp;D39&amp;"&amp;*,ANY',"&amp;E39&amp;");"</f>
+        <f t="shared" ref="G39" si="9">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A39&amp;", '"&amp;B39&amp;"','"&amp;C39&amp;"','"&amp;F39&amp;"?method="&amp;D39&amp;"&amp;*,ANY',"&amp;E39&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (237, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查工作记录详细页面','/AdminEnforceManagerAction.do?method=toAeinspectionDetailPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>238</v>
       </c>
@@ -2156,11 +2278,11 @@
         <v>10</v>
       </c>
       <c r="G40" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A40&amp;", '"&amp;B40&amp;"','"&amp;C40&amp;"','"&amp;F40&amp;"?method="&amp;D40&amp;"&amp;*,ANY',"&amp;E40&amp;");"</f>
+        <f t="shared" ref="G40:G66" si="10">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A40&amp;", '"&amp;B40&amp;"','"&amp;C40&amp;"','"&amp;F40&amp;"?method="&amp;D40&amp;"&amp;*,ANY',"&amp;E40&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (238, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查工作记录修改页面','/AdminEnforceManagerAction.do?method=toUpdateAeinspectionPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>239</v>
       </c>
@@ -2180,11 +2302,11 @@
         <v>10</v>
       </c>
       <c r="G41" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A41&amp;", '"&amp;B41&amp;"','"&amp;C41&amp;"','"&amp;F41&amp;"?method="&amp;D41&amp;"&amp;*,ANY',"&amp;E41&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (239, 'net.sf.jguard.core.authorization.permissions.URLPermission','检查工作记录修改','/AdminEnforceManagerAction.do?method=updateAeinspection&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A42" s="2">
         <v>240</v>
       </c>
@@ -2204,11 +2326,11 @@
         <v>10</v>
       </c>
       <c r="G42" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A42&amp;", '"&amp;B42&amp;"','"&amp;C42&amp;"','"&amp;F42&amp;"?method="&amp;D42&amp;"&amp;*,ANY',"&amp;E42&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (240, 'net.sf.jguard.core.authorization.permissions.URLPermission','检查工作记录删除','/AdminEnforceManagerAction.do?method=delAeinspection&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>241</v>
       </c>
@@ -2228,11 +2350,11 @@
         <v>10</v>
       </c>
       <c r="G43" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A43&amp;", '"&amp;B43&amp;"','"&amp;C43&amp;"','"&amp;F43&amp;"?method="&amp;D43&amp;"&amp;*,ANY',"&amp;E43&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (241, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查结论登记页面','/AdminEnforceManagerAction.do?method=toAeconclusionInitPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>242</v>
       </c>
@@ -2252,11 +2374,11 @@
         <v>10</v>
       </c>
       <c r="G44" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A44&amp;", '"&amp;B44&amp;"','"&amp;C44&amp;"','"&amp;F44&amp;"?method="&amp;D44&amp;"&amp;*,ANY',"&amp;E44&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (242, 'net.sf.jguard.core.authorization.permissions.URLPermission','根据机构No获取用户信息','/AdminEnforceManagerAction.do?method=getUsersByOrgNo&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>243</v>
       </c>
@@ -2276,11 +2398,11 @@
         <v>10</v>
       </c>
       <c r="G45" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A45&amp;", '"&amp;B45&amp;"','"&amp;C45&amp;"','"&amp;F45&amp;"?method="&amp;D45&amp;"&amp;*,ANY',"&amp;E45&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (243, 'net.sf.jguard.core.authorization.permissions.URLPermission','根据机构No获取该机构下子机构','/AdminEnforceManagerAction.do?method=getOrgsByParentOrgNo&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>244</v>
       </c>
@@ -2300,11 +2422,11 @@
         <v>10</v>
       </c>
       <c r="G46" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A46&amp;", '"&amp;B46&amp;"','"&amp;C46&amp;"','"&amp;F46&amp;"?method="&amp;D46&amp;"&amp;*,ANY',"&amp;E46&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (244, 'net.sf.jguard.core.authorization.permissions.URLPermission','检查结论保存方法','/AdminEnforceManagerAction.do?method=createAeconclusion&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>245</v>
       </c>
@@ -2324,11 +2446,11 @@
         <v>10</v>
       </c>
       <c r="G47" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A47&amp;", '"&amp;B47&amp;"','"&amp;C47&amp;"','"&amp;F47&amp;"?method="&amp;D47&amp;"&amp;*,ANY',"&amp;E47&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (245, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查结论列表页面','/AdminEnforceManagerAction.do?method=toAeconclusionList&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>246</v>
       </c>
@@ -2348,11 +2470,11 @@
         <v>10</v>
       </c>
       <c r="G48" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A48&amp;", '"&amp;B48&amp;"','"&amp;C48&amp;"','"&amp;F48&amp;"?method="&amp;D48&amp;"&amp;*,ANY',"&amp;E48&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (246, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查结论详细页面','/AdminEnforceManagerAction.do?method=toAeconclusionDetailPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>247</v>
       </c>
@@ -2372,11 +2494,11 @@
         <v>10</v>
       </c>
       <c r="G49" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A49&amp;", '"&amp;B49&amp;"','"&amp;C49&amp;"','"&amp;F49&amp;"?method="&amp;D49&amp;"&amp;*,ANY',"&amp;E49&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (247, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转检查结论修改页面','/AdminEnforceManagerAction.do?method=toUpdateAeconclusionPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>248</v>
       </c>
@@ -2396,11 +2518,11 @@
         <v>10</v>
       </c>
       <c r="G50" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A50&amp;", '"&amp;B50&amp;"','"&amp;C50&amp;"','"&amp;F50&amp;"?method="&amp;D50&amp;"&amp;*,ANY',"&amp;E50&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (248, 'net.sf.jguard.core.authorization.permissions.URLPermission','检查结论修改','/AdminEnforceManagerAction.do?method=updateAeconclusion&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A51" s="2">
         <v>249</v>
       </c>
@@ -2420,11 +2542,11 @@
         <v>10</v>
       </c>
       <c r="G51" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A51&amp;", '"&amp;B51&amp;"','"&amp;C51&amp;"','"&amp;F51&amp;"?method="&amp;D51&amp;"&amp;*,ANY',"&amp;E51&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (249, 'net.sf.jguard.core.authorization.permissions.URLPermission','检查结论删除','/AdminEnforceManagerAction.do?method=delAeconclusion&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>250</v>
       </c>
@@ -2444,11 +2566,11 @@
         <v>10</v>
       </c>
       <c r="G52" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A52&amp;", '"&amp;B52&amp;"','"&amp;C52&amp;"','"&amp;F52&amp;"?method="&amp;D52&amp;"&amp;*,ANY',"&amp;E52&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (250, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转跟踪整改信息录入页面','/AdminEnforceManagerAction.do?method=toAerectificationInitPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>251</v>
       </c>
@@ -2468,11 +2590,11 @@
         <v>10</v>
       </c>
       <c r="G53" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A53&amp;", '"&amp;B53&amp;"','"&amp;C53&amp;"','"&amp;F53&amp;"?method="&amp;D53&amp;"&amp;*,ANY',"&amp;E53&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (251, 'net.sf.jguard.core.authorization.permissions.URLPermission','跟踪整改信息保存方法','/AdminEnforceManagerAction.do?method=createAerectification&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>252</v>
       </c>
@@ -2492,11 +2614,11 @@
         <v>10</v>
       </c>
       <c r="G54" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A54&amp;", '"&amp;B54&amp;"','"&amp;C54&amp;"','"&amp;F54&amp;"?method="&amp;D54&amp;"&amp;*,ANY',"&amp;E54&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (252, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转跟踪整改信息列表页面','/AdminEnforceManagerAction.do?method=toAerectificationList&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>253</v>
       </c>
@@ -2516,11 +2638,11 @@
         <v>10</v>
       </c>
       <c r="G55" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A55&amp;", '"&amp;B55&amp;"','"&amp;C55&amp;"','"&amp;F55&amp;"?method="&amp;D55&amp;"&amp;*,ANY',"&amp;E55&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (253, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转跟踪整改信息详细页面','/AdminEnforceManagerAction.do?method=toAerectificationDetailPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A56">
         <v>254</v>
       </c>
@@ -2540,11 +2662,11 @@
         <v>10</v>
       </c>
       <c r="G56" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A56&amp;", '"&amp;B56&amp;"','"&amp;C56&amp;"','"&amp;F56&amp;"?method="&amp;D56&amp;"&amp;*,ANY',"&amp;E56&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (254, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转跟踪整改信息修改页面','/AdminEnforceManagerAction.do?method=toUpdateAerectificationPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A57">
         <v>255</v>
       </c>
@@ -2564,11 +2686,11 @@
         <v>10</v>
       </c>
       <c r="G57" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A57&amp;", '"&amp;B57&amp;"','"&amp;C57&amp;"','"&amp;F57&amp;"?method="&amp;D57&amp;"&amp;*,ANY',"&amp;E57&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (255, 'net.sf.jguard.core.authorization.permissions.URLPermission','跟踪整改信息修改','/AdminEnforceManagerAction.do?method=updateAerectification&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A58" s="2">
         <v>256</v>
       </c>
@@ -2588,11 +2710,11 @@
         <v>10</v>
       </c>
       <c r="G58" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A58&amp;", '"&amp;B58&amp;"','"&amp;C58&amp;"','"&amp;F58&amp;"?method="&amp;D58&amp;"&amp;*,ANY',"&amp;E58&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (256, 'net.sf.jguard.core.authorization.permissions.URLPermission','跟踪整改信息删除','/AdminEnforceManagerAction.do?method=delAerectification&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A59">
         <v>258</v>
       </c>
@@ -2612,11 +2734,11 @@
         <v>125</v>
       </c>
       <c r="G59" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A59&amp;", '"&amp;B59&amp;"','"&amp;C59&amp;"','"&amp;F59&amp;"?method="&amp;D59&amp;"&amp;*,ANY',"&amp;E59&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (258, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚信息列表页面','/AdminSanctionManagerAction.do?method=toAeSanctionList&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A60">
         <v>259</v>
       </c>
@@ -2636,11 +2758,11 @@
         <v>125</v>
       </c>
       <c r="G60" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A60&amp;", '"&amp;B60&amp;"','"&amp;C60&amp;"','"&amp;F60&amp;"?method="&amp;D60&amp;"&amp;*,ANY',"&amp;E60&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (259, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚信息登记页面','/AdminSanctionManagerAction.do?method=toAeSanctionInitPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A61">
         <v>260</v>
       </c>
@@ -2660,11 +2782,11 @@
         <v>125</v>
       </c>
       <c r="G61" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A61&amp;", '"&amp;B61&amp;"','"&amp;C61&amp;"','"&amp;F61&amp;"?method="&amp;D61&amp;"&amp;*,ANY',"&amp;E61&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (260, 'net.sf.jguard.core.authorization.permissions.URLPermission','从处罚登记处跳转行政处罚信息登记页面','/AdminSanctionManagerAction.do?method=toAeSanctionInitPageFromPunish&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A62">
         <v>261</v>
       </c>
@@ -2684,11 +2806,11 @@
         <v>125</v>
       </c>
       <c r="G62" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A62&amp;", '"&amp;B62&amp;"','"&amp;C62&amp;"','"&amp;F62&amp;"?method="&amp;D62&amp;"&amp;*,ANY',"&amp;E62&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (261, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政处罚信息保存方法','/AdminSanctionManagerAction.do?method=createAeSanction&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A63">
         <v>262</v>
       </c>
@@ -2708,11 +2830,11 @@
         <v>125</v>
       </c>
       <c r="G63" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A63&amp;", '"&amp;B63&amp;"','"&amp;C63&amp;"','"&amp;F63&amp;"?method="&amp;D63&amp;"&amp;*,ANY',"&amp;E63&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (262, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚信息详细页面','/AdminSanctionManagerAction.do?method=toAeSanctionDetailPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A64">
         <v>263</v>
       </c>
@@ -2732,11 +2854,11 @@
         <v>125</v>
       </c>
       <c r="G64" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A64&amp;", '"&amp;B64&amp;"','"&amp;C64&amp;"','"&amp;F64&amp;"?method="&amp;D64&amp;"&amp;*,ANY',"&amp;E64&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (263, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚信息修改页面','/AdminSanctionManagerAction.do?method=toUpdateAeSanctionPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="65" spans="1:7">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A65">
         <v>264</v>
       </c>
@@ -2756,11 +2878,11 @@
         <v>125</v>
       </c>
       <c r="G65" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A65&amp;", '"&amp;B65&amp;"','"&amp;C65&amp;"','"&amp;F65&amp;"?method="&amp;D65&amp;"&amp;*,ANY',"&amp;E65&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (264, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政处罚信息修改','/AdminSanctionManagerAction.do?method=updateAeSanction&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="66" spans="1:7">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A66" s="2">
         <v>265</v>
       </c>
@@ -2780,11 +2902,11 @@
         <v>125</v>
       </c>
       <c r="G66" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A66&amp;", '"&amp;B66&amp;"','"&amp;C66&amp;"','"&amp;F66&amp;"?method="&amp;D66&amp;"&amp;*,ANY',"&amp;E66&amp;");"</f>
+        <f t="shared" si="10"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (265, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政处罚信息删除','/AdminSanctionManagerAction.do?method=delAeSanction&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="67" spans="1:7">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A67">
         <v>266</v>
       </c>
@@ -2804,11 +2926,11 @@
         <v>125</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" ref="G67" si="9">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A67&amp;", '"&amp;B67&amp;"','"&amp;C67&amp;"','"&amp;F67&amp;"?method="&amp;D67&amp;"&amp;*,ANY',"&amp;E67&amp;");"</f>
+        <f t="shared" ref="G67" si="11">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A67&amp;", '"&amp;B67&amp;"','"&amp;C67&amp;"','"&amp;F67&amp;"?method="&amp;D67&amp;"&amp;*,ANY',"&amp;E67&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (266, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚结论登记页面','/AdminSanctionManagerAction.do?method=toAeSanctionConInitPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="68" spans="1:7">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A68">
         <v>267</v>
       </c>
@@ -2828,11 +2950,11 @@
         <v>125</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" ref="G68" si="10">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A68&amp;", '"&amp;B68&amp;"','"&amp;C68&amp;"','"&amp;F68&amp;"?method="&amp;D68&amp;"&amp;*,ANY',"&amp;E68&amp;");"</f>
+        <f t="shared" ref="G68" si="12">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A68&amp;", '"&amp;B68&amp;"','"&amp;C68&amp;"','"&amp;F68&amp;"?method="&amp;D68&amp;"&amp;*,ANY',"&amp;E68&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (267, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政处罚结论信息保存方法','/AdminSanctionManagerAction.do?method=createAeSanctionCon&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A69">
         <v>268</v>
       </c>
@@ -2852,11 +2974,11 @@
         <v>125</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" ref="G69" si="11">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A69&amp;", '"&amp;B69&amp;"','"&amp;C69&amp;"','"&amp;F69&amp;"?method="&amp;D69&amp;"&amp;*,ANY',"&amp;E69&amp;");"</f>
+        <f t="shared" ref="G69" si="13">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A69&amp;", '"&amp;B69&amp;"','"&amp;C69&amp;"','"&amp;F69&amp;"?method="&amp;D69&amp;"&amp;*,ANY',"&amp;E69&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (268, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚结论信息列表页面','/AdminSanctionManagerAction.do?method=toAeSanctionConList&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="70" spans="1:7">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A70" s="2">
         <v>269</v>
       </c>
@@ -2876,11 +2998,11 @@
         <v>125</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" ref="G70" si="12">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A70&amp;", '"&amp;B70&amp;"','"&amp;C70&amp;"','"&amp;F70&amp;"?method="&amp;D70&amp;"&amp;*,ANY',"&amp;E70&amp;");"</f>
+        <f t="shared" ref="G70" si="14">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A70&amp;", '"&amp;B70&amp;"','"&amp;C70&amp;"','"&amp;F70&amp;"?method="&amp;D70&amp;"&amp;*,ANY',"&amp;E70&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (269, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政处罚结论信息删除','/AdminSanctionManagerAction.do?method=delAeSanctionCon&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="71" spans="1:7">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A71">
         <v>270</v>
       </c>
@@ -2900,11 +3022,11 @@
         <v>125</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" ref="G71:G85" si="13">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A71&amp;", '"&amp;B71&amp;"','"&amp;C71&amp;"','"&amp;F71&amp;"?method="&amp;D71&amp;"&amp;*,ANY',"&amp;E71&amp;");"</f>
+        <f t="shared" ref="G71" si="15">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A71&amp;", '"&amp;B71&amp;"','"&amp;C71&amp;"','"&amp;F71&amp;"?method="&amp;D71&amp;"&amp;*,ANY',"&amp;E71&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (270, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政处罚结论信息详细页面','/AdminSanctionManagerAction.do?method=toAeSanctionConDetailPage&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="72" spans="1:7">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A72">
         <v>271</v>
       </c>
@@ -2924,11 +3046,11 @@
         <v>125</v>
       </c>
       <c r="G72" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A72&amp;", '"&amp;B72&amp;"','"&amp;C72&amp;"','"&amp;F72&amp;"?method="&amp;D72&amp;"&amp;*,ANY',"&amp;E72&amp;");"</f>
+        <f t="shared" ref="G72:G85" si="16">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A72&amp;", '"&amp;B72&amp;"','"&amp;C72&amp;"','"&amp;F72&amp;"?method="&amp;D72&amp;"&amp;*,ANY',"&amp;E72&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (271, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成行政处罚立项审批表Word文件','/AdminSanctionManagerAction.do?method=generateXzcflxbWord&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="73" spans="1:7">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A73">
         <v>272</v>
       </c>
@@ -2948,11 +3070,11 @@
         <v>10</v>
       </c>
       <c r="G73" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A73&amp;", '"&amp;B73&amp;"','"&amp;C73&amp;"','"&amp;F73&amp;"?method="&amp;D73&amp;"&amp;*,ANY',"&amp;E73&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (272, 'net.sf.jguard.core.authorization.permissions.URLPermission','点击登记执法检查结论菜单','/AdminEnforceManagerAction.do?method=toAeinspListForCreateConcl&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="74" spans="1:7">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A74">
         <v>273</v>
       </c>
@@ -2972,11 +3094,11 @@
         <v>10</v>
       </c>
       <c r="G74" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A74&amp;", '"&amp;B74&amp;"','"&amp;C74&amp;"','"&amp;F74&amp;"?method="&amp;D74&amp;"&amp;*,ANY',"&amp;E74&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (273, 'net.sf.jguard.core.authorization.permissions.URLPermission','点击登记执法检查整改记录菜单','/AdminEnforceManagerAction.do?method=toAeinspListForCreateRecti&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="75" spans="1:7">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A75">
         <v>274</v>
       </c>
@@ -2996,11 +3118,11 @@
         <v>10</v>
       </c>
       <c r="G75" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A75&amp;", '"&amp;B75&amp;"','"&amp;C75&amp;"','"&amp;F75&amp;"?method="&amp;D75&amp;"&amp;*,ANY',"&amp;E75&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (274, 'net.sf.jguard.core.authorization.permissions.URLPermission','根据多个机构No获取用户信息','/AdminEnforceManagerAction.do?method=getUsersByOrgNos&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="76" spans="1:7">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A76">
         <v>275</v>
       </c>
@@ -3020,11 +3142,11 @@
         <v>10</v>
       </c>
       <c r="G76" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A76&amp;", '"&amp;B76&amp;"','"&amp;C76&amp;"','"&amp;F76&amp;"?method="&amp;D76&amp;"&amp;*,ANY',"&amp;E76&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (275, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政执法下载附件','/AdminEnforceManagerAction.do?method=downloadAtt&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="77" spans="1:7">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A77">
         <v>276</v>
       </c>
@@ -3044,11 +3166,11 @@
         <v>125</v>
       </c>
       <c r="G77" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A77&amp;", '"&amp;B77&amp;"','"&amp;C77&amp;"','"&amp;F77&amp;"?method="&amp;D77&amp;"&amp;*,ANY',"&amp;E77&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (276, 'net.sf.jguard.core.authorization.permissions.URLPermission','行政处罚下载附件','/AdminSanctionManagerAction.do?method=downloadAtt&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="78" spans="1:7">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A78">
         <v>277</v>
       </c>
@@ -3068,11 +3190,11 @@
         <v>125</v>
       </c>
       <c r="G78" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A78&amp;", '"&amp;B78&amp;"','"&amp;C78&amp;"','"&amp;F78&amp;"?method="&amp;D78&amp;"&amp;*,ANY',"&amp;E78&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (277, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取行政执法结论相关详细信息','/AdminSanctionManagerAction.do?method=getAeconclusionInfo&amp;*,ANY',8);</v>
       </c>
     </row>
-    <row r="79" spans="1:7">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A79" s="3">
         <v>278</v>
       </c>
@@ -3092,11 +3214,11 @@
         <v>125</v>
       </c>
       <c r="G79" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A79&amp;", '"&amp;B79&amp;"','"&amp;C79&amp;"','"&amp;F79&amp;"?method="&amp;D79&amp;"&amp;*,ANY',"&amp;E79&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (278, 'net.sf.jguard.core.authorization.permissions.URLPermission','商业银行获取行政执法结论分页信息','/AdminSanctionManagerAction.do?method=pageAeconclusionInfo&amp;*,ANY',8);</v>
       </c>
     </row>
-    <row r="80" spans="1:7">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A80" s="3">
         <v>284</v>
       </c>
@@ -3116,11 +3238,11 @@
         <v>125</v>
       </c>
       <c r="G80" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A80&amp;", '"&amp;B80&amp;"','"&amp;C80&amp;"','"&amp;F80&amp;"?method="&amp;D80&amp;"&amp;*,ANY',"&amp;E80&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (284, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转商业银行获取行政执法结论分页页面','/AdminSanctionManagerAction.do?method=toPageAeconclusionInfo&amp;*,ANY',8);</v>
       </c>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A81" s="3">
         <v>279</v>
       </c>
@@ -3140,11 +3262,11 @@
         <v>10</v>
       </c>
       <c r="G81" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A81&amp;", '"&amp;B81&amp;"','"&amp;C81&amp;"','"&amp;F81&amp;"?method="&amp;D81&amp;"&amp;*,ANY',"&amp;E81&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (279, 'net.sf.jguard.core.authorization.permissions.URLPermission','根据人民银行机构获取机构下执法人员','/AdminEnforceManagerAction.do?method=getAepeoplesByPcbOrgNo&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A82" s="3">
         <v>280</v>
       </c>
@@ -3164,11 +3286,11 @@
         <v>125</v>
       </c>
       <c r="G82" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A82&amp;", '"&amp;B82&amp;"','"&amp;C82&amp;"','"&amp;F82&amp;"?method="&amp;D82&amp;"&amp;*,ANY',"&amp;E82&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (280, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询系统参数表','/AdminSanctionManagerAction.do?method=pageDctionarys&amp;*,ANY',10);</v>
       </c>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A83" s="3">
         <v>281</v>
       </c>
@@ -3188,11 +3310,11 @@
         <v>125</v>
       </c>
       <c r="G83" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A83&amp;", '"&amp;B83&amp;"','"&amp;C83&amp;"','"&amp;F83&amp;"?method="&amp;D83&amp;"&amp;*,ANY',"&amp;E83&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (281, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存系统参数','/AdminSanctionManagerAction.do?method=saveDctionary&amp;*,ANY',10);</v>
       </c>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A84" s="3">
         <v>282</v>
       </c>
@@ -3212,11 +3334,11 @@
         <v>125</v>
       </c>
       <c r="G84" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A84&amp;", '"&amp;B84&amp;"','"&amp;C84&amp;"','"&amp;F84&amp;"?method="&amp;D84&amp;"&amp;*,ANY',"&amp;E84&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (282, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转系统基础参数设置页面','/AdminSanctionManagerAction.do?method=toSetSystemParam&amp;*,ANY',10);</v>
       </c>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A85" s="4">
         <v>283</v>
       </c>
@@ -3236,11 +3358,11 @@
         <v>125</v>
       </c>
       <c r="G85" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A85&amp;", '"&amp;B85&amp;"','"&amp;C85&amp;"','"&amp;F85&amp;"?method="&amp;D85&amp;"&amp;*,ANY',"&amp;E85&amp;");"</f>
+        <f t="shared" si="16"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (283, 'net.sf.jguard.core.authorization.permissions.URLPermission','删除系统参数','/AdminSanctionManagerAction.do?method=deleteParam&amp;*,ANY',10);</v>
       </c>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A86" s="3">
         <v>285</v>
       </c>
@@ -3260,11 +3382,11 @@
         <v>179</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" ref="G86" si="14">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A86&amp;", '"&amp;B86&amp;"','"&amp;C86&amp;"','"&amp;F86&amp;"?method="&amp;D86&amp;"&amp;*,ANY',"&amp;E86&amp;");"</f>
+        <f t="shared" ref="G86" si="17">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A86&amp;", '"&amp;B86&amp;"','"&amp;C86&amp;"','"&amp;F86&amp;"?method="&amp;D86&amp;"&amp;*,ANY',"&amp;E86&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (285, 'net.sf.jguard.core.authorization.permissions.URLPermission','考试系统管理','/toExam.do?method=toExam&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A87" s="3">
         <v>289</v>
       </c>
@@ -3284,11 +3406,11 @@
         <v>10</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" ref="G87" si="15">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A87&amp;", '"&amp;B87&amp;"','"&amp;C87&amp;"','"&amp;F87&amp;"?method="&amp;D87&amp;"&amp;*,ANY',"&amp;E87&amp;");"</f>
+        <f t="shared" ref="G87" si="18">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A87&amp;", '"&amp;B87&amp;"','"&amp;C87&amp;"','"&amp;F87&amp;"?method="&amp;D87&amp;"&amp;*,ANY',"&amp;E87&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (289, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取登录人当前信息','/AdminEnforceManagerAction.do?method=getLoginInfo&amp;*,ANY',1);</v>
       </c>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A88" s="3">
         <v>290</v>
       </c>
@@ -3308,11 +3430,11 @@
         <v>184</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" ref="G88:G108" si="16">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A88&amp;", '"&amp;B88&amp;"','"&amp;C88&amp;"','"&amp;F88&amp;"?method="&amp;D88&amp;"&amp;*,ANY',"&amp;E88&amp;");"</f>
+        <f t="shared" ref="G88" si="19">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A88&amp;", '"&amp;B88&amp;"','"&amp;C88&amp;"','"&amp;F88&amp;"?method="&amp;D88&amp;"&amp;*,ANY',"&amp;E88&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (290, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转考试成绩导入页面','/ExamAction.do?method=toImportExamScoreExcel&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A89" s="3">
         <v>291</v>
       </c>
@@ -3332,11 +3454,11 @@
         <v>184</v>
       </c>
       <c r="G89" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A89&amp;", '"&amp;B89&amp;"','"&amp;C89&amp;"','"&amp;F89&amp;"?method="&amp;D89&amp;"&amp;*,ANY',"&amp;E89&amp;");"</f>
+        <f t="shared" ref="G89:G108" si="20">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A89&amp;", '"&amp;B89&amp;"','"&amp;C89&amp;"','"&amp;F89&amp;"?method="&amp;D89&amp;"&amp;*,ANY',"&amp;E89&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (291, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转考试成绩列表页面','/ExamAction.do?method=toPageExamScoreInfo&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A90" s="3">
         <v>292</v>
       </c>
@@ -3353,11 +3475,11 @@
         <v>188</v>
       </c>
       <c r="G90" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A90&amp;", '"&amp;B90&amp;"','"&amp;C90&amp;"','"&amp;F90&amp;"?method="&amp;D90&amp;"&amp;*,ANY',"&amp;E90&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (292, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取考试成绩导入进度','/prcscontl.svt?method=&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A91" s="3">
         <v>293</v>
       </c>
@@ -3374,11 +3496,11 @@
         <v>190</v>
       </c>
       <c r="G91" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A91&amp;", '"&amp;B91&amp;"','"&amp;C91&amp;"','"&amp;F91&amp;"?method="&amp;D91&amp;"&amp;*,ANY',"&amp;E91&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (293, 'net.sf.jguard.core.authorization.permissions.URLPermission','考试成绩导入','/trfmlisn.svt?method=&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A92" s="3">
         <v>294</v>
       </c>
@@ -3398,11 +3520,11 @@
         <v>184</v>
       </c>
       <c r="G92" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A92&amp;", '"&amp;B92&amp;"','"&amp;C92&amp;"','"&amp;F92&amp;"?method="&amp;D92&amp;"&amp;*,ANY',"&amp;E92&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (294, 'net.sf.jguard.core.authorization.permissions.URLPermission','查看考试成绩详细信息','/ExamAction.do?method=getExamScoreDetail&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A93">
         <v>295</v>
       </c>
@@ -3422,11 +3544,11 @@
         <v>184</v>
       </c>
       <c r="G93" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A93&amp;", '"&amp;B93&amp;"','"&amp;C93&amp;"','"&amp;F93&amp;"?method="&amp;D93&amp;"&amp;*,ANY',"&amp;E93&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (295, 'net.sf.jguard.core.authorization.permissions.URLPermission','导出考试成绩明细表','/ExamAction.do?method=generateExamScoreAnlExcel&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A94" s="3">
         <v>296</v>
       </c>
@@ -3446,11 +3568,11 @@
         <v>184</v>
       </c>
       <c r="G94" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A94&amp;", '"&amp;B94&amp;"','"&amp;C94&amp;"','"&amp;F94&amp;"?method="&amp;D94&amp;"&amp;*,ANY',"&amp;E94&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (296, 'net.sf.jguard.core.authorization.permissions.URLPermission','查询考试成绩列表','/ExamAction.do?method=pageExamScoreInfo&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A95" s="3">
         <v>297</v>
       </c>
@@ -3470,11 +3592,11 @@
         <v>184</v>
       </c>
       <c r="G95" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A95&amp;", '"&amp;B95&amp;"','"&amp;C95&amp;"','"&amp;F95&amp;"?method="&amp;D95&amp;"&amp;*,ANY',"&amp;E95&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (297, 'net.sf.jguard.core.authorization.permissions.URLPermission','获取考试成绩统计信息','/ExamAction.do?method=getExamScoreAnl&amp;*,ANY',9);</v>
       </c>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A96" s="3">
         <v>298</v>
       </c>
@@ -3494,11 +3616,11 @@
         <v>201</v>
       </c>
       <c r="G96" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A96&amp;", '"&amp;B96&amp;"','"&amp;C96&amp;"','"&amp;F96&amp;"?method="&amp;D96&amp;"&amp;*,ANY',"&amp;E96&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (298, 'net.sf.jguard.core.authorization.permissions.URLPermission','初始化辖内问题概况统计筛选条件页面','/StatisticsAction.do?method=init&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="97" spans="1:7">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A97" s="3">
         <v>299</v>
       </c>
@@ -3518,11 +3640,11 @@
         <v>201</v>
       </c>
       <c r="G97" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A97&amp;", '"&amp;B97&amp;"','"&amp;C97&amp;"','"&amp;F97&amp;"?method="&amp;D97&amp;"&amp;*,ANY',"&amp;E97&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (299, 'net.sf.jguard.core.authorization.permissions.URLPermission','以HTML视图方式展示辖内问题概况统计结果','/StatisticsAction.do?method=displayHtml&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="98" spans="1:7">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A98" s="3">
         <v>300</v>
       </c>
@@ -3542,11 +3664,11 @@
         <v>201</v>
       </c>
       <c r="G98" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A98&amp;", '"&amp;B98&amp;"','"&amp;C98&amp;"','"&amp;F98&amp;"?method="&amp;D98&amp;"&amp;*,ANY',"&amp;E98&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (300, 'net.sf.jguard.core.authorization.permissions.URLPermission','以Excel视图方式展示辖内问题概况统计结果','/StatisticsAction.do?method=displayExcel&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="99" spans="1:7">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A99" s="3">
         <v>301</v>
       </c>
@@ -3566,11 +3688,11 @@
         <v>125</v>
       </c>
       <c r="G99" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A99&amp;", '"&amp;B99&amp;"','"&amp;C99&amp;"','"&amp;F99&amp;"?method="&amp;D99&amp;"&amp;*,ANY',"&amp;E99&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (301, 'net.sf.jguard.core.authorization.permissions.URLPermission','撤销行政处罚信息','/AdminSanctionManagerAction.do?method=repealPunish&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="100" spans="1:7">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A100" s="3">
         <v>302</v>
       </c>
@@ -3590,11 +3712,11 @@
         <v>209</v>
       </c>
       <c r="G100" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A100&amp;", '"&amp;B100&amp;"','"&amp;C100&amp;"','"&amp;F100&amp;"?method="&amp;D100&amp;"&amp;*,ANY',"&amp;E100&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (302, 'net.sf.jguard.core.authorization.permissions.URLPermission','下载公共附件','/FileHandlerManagerAction.do?method=downloadAtt&amp;*,ANY',1);</v>
       </c>
     </row>
-    <row r="101" spans="1:7">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A101" s="3">
         <v>303</v>
       </c>
@@ -3614,11 +3736,11 @@
         <v>10</v>
       </c>
       <c r="G101" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A101&amp;", '"&amp;B101&amp;"','"&amp;C101&amp;"','"&amp;F101&amp;"?method="&amp;D101&amp;"&amp;*,ANY',"&amp;E101&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (303, 'net.sf.jguard.core.authorization.permissions.URLPermission','双击被检查机构树','/AdminEnforceManagerAction.do?method=getAeedOrg&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="102" spans="1:7">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A102" s="3">
         <v>304</v>
       </c>
@@ -3638,11 +3760,11 @@
         <v>10</v>
       </c>
       <c r="G102" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A102&amp;", '"&amp;B102&amp;"','"&amp;C102&amp;"','"&amp;F102&amp;"?method="&amp;D102&amp;"&amp;*,ANY',"&amp;E102&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (304, 'net.sf.jguard.core.authorization.permissions.URLPermission','选择涉及机构下属机构','/AdminEnforceManagerAction.do?method=selectChildInvolveBank&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="103" spans="1:7">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A103" s="3">
         <v>305</v>
       </c>
@@ -3662,11 +3784,11 @@
         <v>10</v>
       </c>
       <c r="G103" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A103&amp;", '"&amp;B103&amp;"','"&amp;C103&amp;"','"&amp;F103&amp;"?method="&amp;D103&amp;"&amp;*,ANY',"&amp;E103&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (305, 'net.sf.jguard.core.authorization.permissions.URLPermission','选择涉及机构下属机构包含自己','/AdminEnforceManagerAction.do?method=getOrgsByParentOrgNoContainSelf&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="104" spans="1:7">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A104" s="3">
         <v>306</v>
       </c>
@@ -3686,11 +3808,11 @@
         <v>10</v>
       </c>
       <c r="G104" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A104&amp;", '"&amp;B104&amp;"','"&amp;C104&amp;"','"&amp;F104&amp;"?method="&amp;D104&amp;"&amp;*,ANY',"&amp;E104&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (306, 'net.sf.jguard.core.authorization.permissions.URLPermission','判断是否已经录入工作检查记录','/AdminEnforceManagerAction.do?method=isExsitAeInspc&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="105" spans="1:7">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A105" s="3">
         <v>307</v>
       </c>
@@ -3710,11 +3832,11 @@
         <v>10</v>
       </c>
       <c r="G105" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A105&amp;", '"&amp;B105&amp;"','"&amp;C105&amp;"','"&amp;F105&amp;"?method="&amp;D105&amp;"&amp;*,ANY',"&amp;E105&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (307, 'net.sf.jguard.core.authorization.permissions.URLPermission','删除工作底稿检查详情','/AdminEnforceManagerAction.do?method=deleteBasis&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A106" s="3">
         <v>308</v>
       </c>
@@ -3734,11 +3856,11 @@
         <v>10</v>
       </c>
       <c r="G106" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A106&amp;", '"&amp;B106&amp;"','"&amp;C106&amp;"','"&amp;F106&amp;"?method="&amp;D106&amp;"&amp;*,ANY',"&amp;E106&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (308, 'net.sf.jguard.core.authorization.permissions.URLPermission','判断是否已经完成了所有相关工作内容','/AdminEnforceManagerAction.do?method=isInputAllWork&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A107" s="3">
         <v>309</v>
       </c>
@@ -3758,11 +3880,11 @@
         <v>10</v>
       </c>
       <c r="G107" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A107&amp;", '"&amp;B107&amp;"','"&amp;C107&amp;"','"&amp;F107&amp;"?method="&amp;D107&amp;"&amp;*,ANY',"&amp;E107&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (309, 'net.sf.jguard.core.authorization.permissions.URLPermission','修改检查工作记录时保存工作底稿','/AdminEnforceManagerAction.do?method=saveBasisAtUpdateInspc&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A108">
         <v>310</v>
       </c>
@@ -3782,11 +3904,11 @@
         <v>10</v>
       </c>
       <c r="G108" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A108&amp;", '"&amp;B108&amp;"','"&amp;C108&amp;"','"&amp;F108&amp;"?method="&amp;D108&amp;"&amp;*,ANY',"&amp;E108&amp;");"</f>
+        <f t="shared" si="20"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (310, 'net.sf.jguard.core.authorization.permissions.URLPermission','分页查询事实认定书','/AdminEnforceManagerAction.do?method=pageFactBook&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A109">
         <v>311</v>
       </c>
@@ -3806,11 +3928,11 @@
         <v>10</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" ref="G109:G117" si="17">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A109&amp;", '"&amp;B109&amp;"','"&amp;C109&amp;"','"&amp;F109&amp;"?method="&amp;D109&amp;"&amp;*,ANY',"&amp;E109&amp;");"</f>
+        <f t="shared" ref="G109" si="21">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A109&amp;", '"&amp;B109&amp;"','"&amp;C109&amp;"','"&amp;F109&amp;"?method="&amp;D109&amp;"&amp;*,ANY',"&amp;E109&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (311, 'net.sf.jguard.core.authorization.permissions.URLPermission','查询导出数据到ms-excel文件','/AdminEnforceManagerAction.do?method=exportXls&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A110">
         <v>312</v>
       </c>
@@ -3830,11 +3952,11 @@
         <v>10</v>
       </c>
       <c r="G110" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A110&amp;", '"&amp;B110&amp;"','"&amp;C110&amp;"','"&amp;F110&amp;"?method="&amp;D110&amp;"&amp;*,ANY',"&amp;E110&amp;");"</f>
+        <f t="shared" ref="G110:G126" si="22">"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A110&amp;", '"&amp;B110&amp;"','"&amp;C110&amp;"','"&amp;F110&amp;"?method="&amp;D110&amp;"&amp;*,ANY',"&amp;E110&amp;");"</f>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (312, 'net.sf.jguard.core.authorization.permissions.URLPermission','生成行政执法检查情况统计表Excel文件','/AdminEnforceManagerAction.do?method=generateAeFeedBackExcel&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A111">
         <v>313</v>
       </c>
@@ -3854,11 +3976,11 @@
         <v>125</v>
       </c>
       <c r="G111" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A111&amp;", '"&amp;B111&amp;"','"&amp;C111&amp;"','"&amp;F111&amp;"?method="&amp;D111&amp;"&amp;*,ANY',"&amp;E111&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (313, 'net.sf.jguard.core.authorization.permissions.URLPermission','初始化录入检查结论反馈页面','/AdminSanctionManagerAction.do?method=getFeedbackInfo&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A112">
         <v>314</v>
       </c>
@@ -3878,11 +4000,11 @@
         <v>125</v>
       </c>
       <c r="G112" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A112&amp;", '"&amp;B112&amp;"','"&amp;C112&amp;"','"&amp;F112&amp;"?method="&amp;D112&amp;"&amp;*,ANY',"&amp;E112&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (314, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存检查结论反馈意见','/AdminSanctionManagerAction.do?method=saveFeedBack&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="113" spans="1:7">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A113">
         <v>315</v>
       </c>
@@ -3902,11 +4024,11 @@
         <v>125</v>
       </c>
       <c r="G113" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A113&amp;", '"&amp;B113&amp;"','"&amp;C113&amp;"','"&amp;F113&amp;"?method="&amp;D113&amp;"&amp;*,ANY',"&amp;E113&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (315, 'net.sf.jguard.core.authorization.permissions.URLPermission','初始化录入行政处罚反馈页面','/AdminSanctionManagerAction.do?method=getPublishFeedbackInfo&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="114" spans="1:7">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A114">
         <v>316</v>
       </c>
@@ -3926,11 +4048,11 @@
         <v>125</v>
       </c>
       <c r="G114" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A114&amp;", '"&amp;B114&amp;"','"&amp;C114&amp;"','"&amp;F114&amp;"?method="&amp;D114&amp;"&amp;*,ANY',"&amp;E114&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (316, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存行政处罚反馈意见','/AdminSanctionManagerAction.do?method=savePublishFeedBack&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="115" spans="1:7">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A115">
         <v>317</v>
       </c>
@@ -3950,11 +4072,11 @@
         <v>201</v>
       </c>
       <c r="G115" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A115&amp;", '"&amp;B115&amp;"','"&amp;C115&amp;"','"&amp;F115&amp;"?method="&amp;D115&amp;"&amp;*,ANY',"&amp;E115&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (317, 'net.sf.jguard.core.authorization.permissions.URLPermission','初始化反馈意见统计筛选条件页面','/StatisticsAction.do?method=initFeedback&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="116" spans="1:7">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A116">
         <v>318</v>
       </c>
@@ -3974,11 +4096,11 @@
         <v>201</v>
       </c>
       <c r="G116" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A116&amp;", '"&amp;B116&amp;"','"&amp;C116&amp;"','"&amp;F116&amp;"?method="&amp;D116&amp;"&amp;*,ANY',"&amp;E116&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (318, 'net.sf.jguard.core.authorization.permissions.URLPermission','以HTML视图方式展示反馈意见统计结果','/StatisticsAction.do?method=displayFeedbackHtml&amp;*,ANY',5);</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A117">
         <v>319</v>
       </c>
@@ -3998,13 +4120,230 @@
         <v>201</v>
       </c>
       <c r="G117" t="str">
-        <f>"INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES ("&amp;A117&amp;", '"&amp;B117&amp;"','"&amp;C117&amp;"','"&amp;F117&amp;"?method="&amp;D117&amp;"&amp;*,ANY',"&amp;E117&amp;");"</f>
+        <f t="shared" si="22"/>
         <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (319, 'net.sf.jguard.core.authorization.permissions.URLPermission','以Excel视图方式展示反馈意见统计结果','/StatisticsAction.do?method=displayFeedbackExcel&amp;*,ANY',5);</v>
       </c>
     </row>
+    <row r="118" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A118">
+        <v>320</v>
+      </c>
+      <c r="B118" t="s">
+        <v>7</v>
+      </c>
+      <c r="C118" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="D118" t="s">
+        <v>243</v>
+      </c>
+      <c r="E118">
+        <v>5</v>
+      </c>
+      <c r="F118" t="s">
+        <v>10</v>
+      </c>
+      <c r="G118" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (320, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转到筛选执法人员和被检查机构页面','/AdminEnforceManagerAction.do?method=toSiftPage&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A119">
+        <v>321</v>
+      </c>
+      <c r="B119" t="s">
+        <v>7</v>
+      </c>
+      <c r="C119" t="s">
+        <v>259</v>
+      </c>
+      <c r="D119" t="s">
+        <v>244</v>
+      </c>
+      <c r="E119">
+        <v>5</v>
+      </c>
+      <c r="F119" t="s">
+        <v>10</v>
+      </c>
+      <c r="G119" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (321, 'net.sf.jguard.core.authorization.permissions.URLPermission','筛选其他组成员','/AdminEnforceManagerAction.do?method=siftAePeoples&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A120">
+        <v>322</v>
+      </c>
+      <c r="B120" t="s">
+        <v>7</v>
+      </c>
+      <c r="C120" t="s">
+        <v>258</v>
+      </c>
+      <c r="D120" t="s">
+        <v>245</v>
+      </c>
+      <c r="E120">
+        <v>5</v>
+      </c>
+      <c r="F120" t="s">
+        <v>10</v>
+      </c>
+      <c r="G120" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (322, 'net.sf.jguard.core.authorization.permissions.URLPermission','筛选被检查机构','/AdminEnforceManagerAction.do?method=siftAeedOrg&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A121">
+        <v>323</v>
+      </c>
+      <c r="B121" t="s">
+        <v>7</v>
+      </c>
+      <c r="C121" t="s">
+        <v>257</v>
+      </c>
+      <c r="D121" t="s">
+        <v>246</v>
+      </c>
+      <c r="E121">
+        <v>5</v>
+      </c>
+      <c r="F121" t="s">
+        <v>10</v>
+      </c>
+      <c r="G121" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (323, 'net.sf.jguard.core.authorization.permissions.URLPermission','保存筛选结果','/AdminEnforceManagerAction.do?method=toAdminEnforceInitPageFromSift&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A122">
+        <v>324</v>
+      </c>
+      <c r="B122" t="s">
+        <v>7</v>
+      </c>
+      <c r="C122" t="s">
+        <v>256</v>
+      </c>
+      <c r="D122" t="s">
+        <v>247</v>
+      </c>
+      <c r="E122">
+        <v>5</v>
+      </c>
+      <c r="F122" t="s">
+        <v>10</v>
+      </c>
+      <c r="G122" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (324, 'net.sf.jguard.core.authorization.permissions.URLPermission','筛选结果列表页面','/AdminEnforceManagerAction.do?method=toSiftResultList&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A123">
+        <v>325</v>
+      </c>
+      <c r="B123" t="s">
+        <v>7</v>
+      </c>
+      <c r="C123" t="s">
+        <v>255</v>
+      </c>
+      <c r="D123" t="s">
+        <v>248</v>
+      </c>
+      <c r="E123">
+        <v>5</v>
+      </c>
+      <c r="F123" t="s">
+        <v>10</v>
+      </c>
+      <c r="G123" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (325, 'net.sf.jguard.core.authorization.permissions.URLPermission','从筛选结果跳转行政执法登记页面','/AdminEnforceManagerAction.do?method=toAdminEnforceInitPageFromSiftResult&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A124">
+        <v>326</v>
+      </c>
+      <c r="B124" t="s">
+        <v>7</v>
+      </c>
+      <c r="C124" t="s">
+        <v>254</v>
+      </c>
+      <c r="D124" t="s">
+        <v>249</v>
+      </c>
+      <c r="E124">
+        <v>5</v>
+      </c>
+      <c r="F124" t="s">
+        <v>10</v>
+      </c>
+      <c r="G124" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (326, 'net.sf.jguard.core.authorization.permissions.URLPermission','导出单机版初始化文件','/AdminEnforceManagerAction.do?method=generateDesktopClientInitialFile&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A125">
+        <v>327</v>
+      </c>
+      <c r="B125" t="s">
+        <v>7</v>
+      </c>
+      <c r="C125" t="s">
+        <v>253</v>
+      </c>
+      <c r="D125" t="s">
+        <v>250</v>
+      </c>
+      <c r="E125">
+        <v>5</v>
+      </c>
+      <c r="F125" t="s">
+        <v>10</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (327, 'net.sf.jguard.core.authorization.permissions.URLPermission','跳转行政执法的工作检查记录单机版数据导入界面','/AdminEnforceManagerAction.do?method=toImportDesktopClientFinalData&amp;*,ANY',5);</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A126">
+        <v>328</v>
+      </c>
+      <c r="B126" t="s">
+        <v>7</v>
+      </c>
+      <c r="C126" t="s">
+        <v>252</v>
+      </c>
+      <c r="D126" t="s">
+        <v>251</v>
+      </c>
+      <c r="E126">
+        <v>5</v>
+      </c>
+      <c r="F126" t="s">
+        <v>10</v>
+      </c>
+      <c r="G126" t="str">
+        <f t="shared" si="22"/>
+        <v>INSERT INTO JG_PERMISSION (ID, CLASS, NAME, ACTIONS, DOMAIN_ID) VALUES (328, 'net.sf.jguard.core.authorization.permissions.URLPermission','导入行政执法的工作检查记录单机版数据','/AdminEnforceManagerAction.do?method=importDesktopClientFinalData&amp;*,ANY',5);</v>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300"/>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>